<commit_message>
Changed the reports to the right sp
</commit_message>
<xml_diff>
--- a/R/data/df_persona_per_group.xlsx
+++ b/R/data/df_persona_per_group.xlsx
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D2">
-        <v>502</v>
+        <v>915</v>
       </c>
       <c r="E2">
-        <v>0.18</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -595,34 +595,34 @@
         </is>
       </c>
       <c r="R2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="T2">
-        <v>39.8</v>
+        <v>32.4</v>
       </c>
       <c r="U2">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V2">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W2">
+        <v>5.9</v>
+      </c>
+      <c r="X2">
         <v>6.3</v>
       </c>
-      <c r="X2">
-        <v>6.5</v>
-      </c>
       <c r="Y2">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z2">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB2">
         <v>0</v>
@@ -646,13 +646,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D3">
-        <v>2280</v>
+        <v>698</v>
       </c>
       <c r="E3">
-        <v>0.82</v>
+        <v>0.433</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>EM&amp;CM</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -718,28 +718,28 @@
         <v>19</v>
       </c>
       <c r="S3">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="T3">
-        <v>44.2</v>
+        <v>33.4</v>
       </c>
       <c r="U3">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V3">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W3">
+        <v>5.9</v>
+      </c>
+      <c r="X3">
         <v>6.3</v>
       </c>
-      <c r="X3">
-        <v>6.5</v>
-      </c>
       <c r="Y3">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z3">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA3">
         <v>0.1</v>
@@ -751,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="AD3">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="4">
@@ -766,17 +766,17 @@
         </is>
       </c>
       <c r="C4">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D4">
-        <v>1176</v>
+        <v>756</v>
       </c>
       <c r="E4">
-        <v>0.423</v>
+        <v>0.469</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>MedV</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -801,12 +801,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -835,37 +835,37 @@
         </is>
       </c>
       <c r="R4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S4">
-        <v>145</v>
+        <v>137.5</v>
       </c>
       <c r="T4">
-        <v>46</v>
+        <v>34.2</v>
       </c>
       <c r="U4">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V4">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W4">
+        <v>5.9</v>
+      </c>
+      <c r="X4">
         <v>6.3</v>
       </c>
-      <c r="X4">
-        <v>6.5</v>
-      </c>
       <c r="Y4">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z4">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA4">
         <v>0.1</v>
       </c>
       <c r="AB4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -886,13 +886,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D5">
-        <v>428</v>
+        <v>176</v>
       </c>
       <c r="E5">
-        <v>0.154</v>
+        <v>0.109</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>MedV</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -958,31 +958,31 @@
         <v>20</v>
       </c>
       <c r="S5">
-        <v>133.5</v>
+        <v>134.5</v>
       </c>
       <c r="T5">
-        <v>42.4</v>
+        <v>34.7</v>
       </c>
       <c r="U5">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V5">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W5">
+        <v>5.9</v>
+      </c>
+      <c r="X5">
         <v>6.3</v>
       </c>
-      <c r="X5">
-        <v>6.5</v>
-      </c>
       <c r="Y5">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z5">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB5">
         <v>0</v>
@@ -991,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="AD5">
-        <v>2016.5</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="6">
@@ -1006,17 +1006,17 @@
         </is>
       </c>
       <c r="C6">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D6">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="E6">
-        <v>0.062</v>
+        <v>0.125</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ZW</t>
+          <t>EM&amp;CM</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1046,17 +1046,17 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1075,31 +1075,31 @@
         </is>
       </c>
       <c r="R6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S6">
-        <v>125</v>
+        <v>128.5</v>
       </c>
       <c r="T6">
-        <v>27.9</v>
+        <v>28.1</v>
       </c>
       <c r="U6">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V6">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W6">
+        <v>5.9</v>
+      </c>
+      <c r="X6">
         <v>6.3</v>
       </c>
-      <c r="X6">
-        <v>6.5</v>
-      </c>
       <c r="Y6">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z6">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="AD6">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="7">
@@ -1126,17 +1126,17 @@
         </is>
       </c>
       <c r="C7">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D7">
-        <v>912</v>
+        <v>445</v>
       </c>
       <c r="E7">
-        <v>0.328</v>
+        <v>0.276</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1195,31 +1195,31 @@
         </is>
       </c>
       <c r="R7">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S7">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="T7">
-        <v>45.6</v>
+        <v>36.1</v>
       </c>
       <c r="U7">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V7">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W7">
+        <v>5.9</v>
+      </c>
+      <c r="X7">
         <v>6.3</v>
       </c>
-      <c r="X7">
-        <v>6.5</v>
-      </c>
       <c r="Y7">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z7">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA7">
         <v>0</v>
@@ -1246,112 +1246,112 @@
         </is>
       </c>
       <c r="C8">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2e Studie</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>HAVO</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>EM</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="R8">
         <v>22</v>
       </c>
-      <c r="E8">
-        <v>0.008</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2e Studie</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>HAVO</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>NG</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Nee</t>
-        </is>
-      </c>
-      <c r="R8">
-        <v>21</v>
-      </c>
       <c r="S8">
-        <v>172.5</v>
+        <v>60</v>
       </c>
       <c r="T8">
-        <v>25.8</v>
+        <v>29.8</v>
       </c>
       <c r="U8">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V8">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W8">
+        <v>5.9</v>
+      </c>
+      <c r="X8">
         <v>6.3</v>
       </c>
-      <c r="X8">
-        <v>6.5</v>
-      </c>
       <c r="Y8">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z8">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA8">
         <v>0</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC8">
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="9">
@@ -1366,17 +1366,17 @@
         </is>
       </c>
       <c r="C9">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D9">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="E9">
-        <v>0.026</v>
+        <v>0.012</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>EM&amp;CM</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1438,28 +1438,28 @@
         <v>22</v>
       </c>
       <c r="S9">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T9">
-        <v>45.3</v>
+        <v>30.5</v>
       </c>
       <c r="U9">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V9">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W9">
+        <v>5.9</v>
+      </c>
+      <c r="X9">
         <v>6.3</v>
       </c>
-      <c r="X9">
-        <v>6.5</v>
-      </c>
       <c r="Y9">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z9">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="AD9">
-        <v>2019</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="10">
@@ -1486,17 +1486,17 @@
         </is>
       </c>
       <c r="C10">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D10">
-        <v>721</v>
+        <v>522</v>
       </c>
       <c r="E10">
-        <v>0.259</v>
+        <v>0.324</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>ZW</t>
+          <t>MedV</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1558,28 +1558,28 @@
         <v>21</v>
       </c>
       <c r="S10">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="T10">
-        <v>39.4</v>
+        <v>32.7</v>
       </c>
       <c r="U10">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V10">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W10">
+        <v>5.9</v>
+      </c>
+      <c r="X10">
         <v>6.3</v>
       </c>
-      <c r="X10">
-        <v>6.5</v>
-      </c>
       <c r="Y10">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z10">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="AD10">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="11">
@@ -1606,17 +1606,17 @@
         </is>
       </c>
       <c r="C11">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D11">
-        <v>1478</v>
+        <v>860</v>
       </c>
       <c r="E11">
-        <v>0.531</v>
+        <v>0.533</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>EM&amp;CM</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1678,34 +1678,34 @@
         <v>19</v>
       </c>
       <c r="S11">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="T11">
-        <v>45.6</v>
+        <v>35.9</v>
       </c>
       <c r="U11">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V11">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W11">
+        <v>5.9</v>
+      </c>
+      <c r="X11">
         <v>6.3</v>
       </c>
-      <c r="X11">
-        <v>6.5</v>
-      </c>
       <c r="Y11">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z11">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA11">
         <v>0.1</v>
       </c>
       <c r="AB11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1726,17 +1726,17 @@
         </is>
       </c>
       <c r="C12">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D12">
-        <v>192</v>
+        <v>58</v>
       </c>
       <c r="E12">
-        <v>0.06900000000000001</v>
+        <v>0.036</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>EM</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1798,28 +1798,28 @@
         <v>19</v>
       </c>
       <c r="S12">
-        <v>128.5</v>
+        <v>132</v>
       </c>
       <c r="T12">
-        <v>47.2</v>
+        <v>30.9</v>
       </c>
       <c r="U12">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V12">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W12">
+        <v>5.9</v>
+      </c>
+      <c r="X12">
         <v>6.3</v>
       </c>
-      <c r="X12">
-        <v>6.5</v>
-      </c>
       <c r="Y12">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z12">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA12">
         <v>0.1</v>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="AD12">
-        <v>2014</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="13">
@@ -1846,22 +1846,22 @@
         </is>
       </c>
       <c r="C13">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D13">
-        <v>159</v>
+        <v>92</v>
       </c>
       <c r="E13">
         <v>0.057</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Tussenjaar</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1918,28 +1918,28 @@
         <v>21</v>
       </c>
       <c r="S13">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="T13">
-        <v>29.5</v>
+        <v>15.5</v>
       </c>
       <c r="U13">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V13">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W13">
+        <v>5.9</v>
+      </c>
+      <c r="X13">
         <v>6.3</v>
       </c>
-      <c r="X13">
-        <v>6.5</v>
-      </c>
       <c r="Y13">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z13">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA13">
         <v>0</v>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="AD13">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="14">
@@ -1966,17 +1966,17 @@
         </is>
       </c>
       <c r="C14">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D14">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="E14">
-        <v>0.028</v>
+        <v>0.019</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -2038,40 +2038,40 @@
         <v>22</v>
       </c>
       <c r="S14">
-        <v>131</v>
+        <v>127.5</v>
       </c>
       <c r="T14">
-        <v>45.3</v>
+        <v>29.6</v>
       </c>
       <c r="U14">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V14">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W14">
+        <v>5.9</v>
+      </c>
+      <c r="X14">
         <v>6.3</v>
       </c>
-      <c r="X14">
-        <v>6.5</v>
-      </c>
       <c r="Y14">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z14">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA14">
         <v>0</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>2018</v>
+        <v>2017.5</v>
       </c>
     </row>
     <row r="15">
@@ -2086,13 +2086,13 @@
         </is>
       </c>
       <c r="C15">
-        <v>2782</v>
+        <v>1613</v>
       </c>
       <c r="D15">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="E15">
-        <v>0.056</v>
+        <v>0.032</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2155,43 +2155,43 @@
         </is>
       </c>
       <c r="R15">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S15">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="T15">
-        <v>46</v>
+        <v>38.3</v>
       </c>
       <c r="U15">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="V15">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="W15">
+        <v>5.9</v>
+      </c>
+      <c r="X15">
         <v>6.3</v>
       </c>
-      <c r="X15">
-        <v>6.5</v>
-      </c>
       <c r="Y15">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="Z15">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="AA15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>